<commit_message>
Update Japan country data in HEART Model Excel file
</commit_message>
<xml_diff>
--- a/data/HEART_Model_khurshidOGcleaned.xlsx
+++ b/data/HEART_Model_khurshidOGcleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Personal\Working on It\Eco\finalproduct\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55558666-8835-4E8E-B4E1-F94D4097DCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A33E526-3586-47D6-9E01-FAF3B9927C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-86" yWindow="0" windowWidth="11143" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEART" sheetId="1" r:id="rId1"/>
@@ -272,9 +272,6 @@
     <t>JAPAN</t>
   </si>
   <si>
-    <t>0.41B-</t>
-  </si>
-  <si>
     <t>5th largest per GDP. Facing growth,ageing population and US threat challenges.</t>
   </si>
   <si>
@@ -570,13 +567,16 @@
   </si>
   <si>
     <t>South Africa currently has the largest economy in Africa. The country is a permanent member of G-20 and recently hosted annual G-20 summit in Johannesburg. South Africa is a mid-sized global economy with over $426 billions of GDP nominal representing 0.37% of the global economy also reflecting a relatively small but regionally influential economic presence.</t>
+  </si>
+  <si>
+    <t>0.35B-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="13">
+  <numFmts count="12">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@"/>
@@ -586,10 +586,9 @@
     <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="185" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="0.000"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -913,10 +912,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1057,10 +1056,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="185" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1290,10 +1289,10 @@
   <dimension ref="A1:AP24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AL18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AP8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="AP13" sqref="AP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1344,13 +1343,13 @@
   <sheetData>
     <row r="1" spans="1:42" ht="14.15">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -2944,7 +2943,6 @@
     </row>
     <row r="13" spans="1:42" ht="33.9">
       <c r="A13" s="26">
-        <f t="shared" si="21"/>
         <v>11</v>
       </c>
       <c r="B13" s="27" t="s">
@@ -2952,6 +2950,7 @@
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="14">
+        <f>4186000000000</f>
         <v>4186000000000</v>
       </c>
       <c r="E13" s="28">
@@ -2984,26 +2983,28 @@
         <v>2.75E-2</v>
       </c>
       <c r="N13" s="14">
-        <v>1758120000000</v>
+        <f>10255700000000</f>
+        <v>10255700000000</v>
       </c>
       <c r="O13" s="14">
         <f t="shared" si="4"/>
-        <v>48348300000</v>
+        <v>282031750000</v>
       </c>
       <c r="P13" s="14">
         <f t="shared" si="5"/>
-        <v>1806468300000</v>
+        <v>10537731750000</v>
       </c>
       <c r="Q13" s="29">
         <f t="shared" si="6"/>
-        <v>1.155E-2</v>
+        <v>6.7375000000000004E-2</v>
       </c>
       <c r="R13" s="30">
         <f t="shared" si="7"/>
-        <v>0.43154999999999999</v>
+        <v>2.5173749999999999</v>
       </c>
       <c r="S13" s="12"/>
       <c r="T13" s="14">
+        <f>1385000000000</f>
         <v>1385000000000</v>
       </c>
       <c r="U13" s="30">
@@ -3022,6 +3023,7 @@
         <v>-1.9111323459149545E-3</v>
       </c>
       <c r="Y13" s="14">
+        <f>460460000000</f>
         <v>460460000000</v>
       </c>
       <c r="Z13" s="29">
@@ -3029,13 +3031,14 @@
         <v>0.11</v>
       </c>
       <c r="AA13" s="36">
-        <v>65099999.999999993</v>
+        <v>65100000</v>
       </c>
       <c r="AB13" s="37">
         <f t="shared" si="12"/>
         <v>0.52755267423014585</v>
       </c>
       <c r="AC13" s="38">
+        <f>502320000000</f>
         <v>502320000000</v>
       </c>
       <c r="AD13" s="29">
@@ -3050,6 +3053,7 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="AG13" s="31">
+        <f>221858000000</f>
         <v>221858000000</v>
       </c>
       <c r="AH13" s="29">
@@ -3058,7 +3062,7 @@
       </c>
       <c r="AI13" s="39">
         <f t="shared" si="16"/>
-        <v>0.40932409599992786</v>
+        <v>0.35349909599992785</v>
       </c>
       <c r="AJ13" s="40">
         <v>0.93899999999999995</v>
@@ -3078,10 +3082,10 @@
         <v>74</v>
       </c>
       <c r="AO13" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP13" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="AP13" s="13" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:42" ht="33.9">
@@ -3090,7 +3094,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="14">
@@ -3220,10 +3224,10 @@
         <v>74</v>
       </c>
       <c r="AO14" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP14" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="AP14" s="13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:42" ht="33.9">
@@ -3231,7 +3235,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="14">
@@ -3361,10 +3365,10 @@
         <v>74</v>
       </c>
       <c r="AO15" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP15" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="AP15" s="13" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:42" ht="33.9">
@@ -3373,7 +3377,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="14">
@@ -3500,13 +3504,13 @@
         <v>28532.028571428578</v>
       </c>
       <c r="AN16" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO16" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="AO16" s="45" t="s">
+      <c r="AP16" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="AP16" s="13" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:42" ht="33.9">
@@ -3515,7 +3519,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="14">
@@ -3642,13 +3646,13 @@
         <v>32143.727789165441</v>
       </c>
       <c r="AN17" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO17" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="AO17" s="45" t="s">
+      <c r="AP17" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="AP17" s="13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:42" ht="33.9">
@@ -3657,7 +3661,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="14">
@@ -3784,13 +3788,13 @@
         <v>33939.027363166664</v>
       </c>
       <c r="AN18" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AO18" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP18" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="AP18" s="13" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:42" ht="33.9">
@@ -3798,7 +3802,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="14">
@@ -3925,13 +3929,13 @@
         <v>37028.409090909088</v>
       </c>
       <c r="AN19" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="AO19" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="AO19" s="45" t="s">
+      <c r="AP19" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="AP19" s="13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:42" ht="33.9">
@@ -3940,7 +3944,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="14">
@@ -4067,13 +4071,13 @@
         <v>39300.546523297482</v>
       </c>
       <c r="AN20" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO20" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP20" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="AP20" s="13" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:42" ht="33.9">
@@ -4082,7 +4086,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="14">
@@ -4212,10 +4216,10 @@
         <v>42</v>
       </c>
       <c r="AO21" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP21" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="AP21" s="13" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:42" ht="33.9">
@@ -4224,7 +4228,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="14">
@@ -4351,13 +4355,13 @@
         <v>68163.18681318681</v>
       </c>
       <c r="AN22" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO22" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="AO22" s="45" t="s">
+      <c r="AP22" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="AP22" s="13" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:42" ht="33.9">
@@ -4366,7 +4370,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="74">
@@ -4496,10 +4500,10 @@
         <v>53</v>
       </c>
       <c r="AO23" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AP23" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:42" ht="33.9">
@@ -4508,7 +4512,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="14">
@@ -4638,15 +4642,16 @@
         <v>46</v>
       </c>
       <c r="AO24" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AP24" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4666,18 +4671,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="71" t="s">
         <v>152</v>
-      </c>
-      <c r="B1" s="71" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
         <v>150</v>
-      </c>
-      <c r="B2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4685,15 +4690,15 @@
         <v>0</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
         <v>155</v>
-      </c>
-      <c r="B4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4701,7 +4706,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4709,7 +4714,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4923,16 +4928,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="C1" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="48" t="s">
-        <v>131</v>
-      </c>
       <c r="D1" s="48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4940,13 +4945,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="50" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4954,13 +4959,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4968,13 +4973,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="51" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4982,13 +4987,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="51" t="s">
-        <v>136</v>
-      </c>
       <c r="D5" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4996,13 +5001,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" s="51" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5010,13 +5015,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="51" t="s">
-        <v>139</v>
-      </c>
       <c r="D7" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5024,13 +5029,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5038,13 +5043,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5052,13 +5057,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5066,13 +5071,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5080,13 +5085,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5094,13 +5099,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -5128,65 +5133,65 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="56"/>
       <c r="D1" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="56">
         <v>0.59</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="56">
         <v>0.44650000000000001</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="56">
         <v>0.15129999999999999</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="56">
         <v>33.880000000000003</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" s="56">
         <v>80.89</v>
@@ -5194,7 +5199,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="67"/>
     </row>
@@ -5204,50 +5209,50 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="67" t="s">
         <v>123</v>
-      </c>
-      <c r="B12" s="67" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="56" t="s">
         <v>125</v>
-      </c>
-      <c r="B13" s="56" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="56" t="s">
         <v>127</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>